<commit_message>
Creating more powerful recipe search function
</commit_message>
<xml_diff>
--- a/Ingredients.xlsx
+++ b/Ingredients.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="171">
   <si>
     <t xml:space="preserve">Recipe</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">flour oat or almond</t>
   </si>
   <si>
-    <t xml:space="preserve">parsely</t>
+    <t xml:space="preserve">parsley</t>
   </si>
   <si>
     <t xml:space="preserve">0.25 cup</t>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Chipotle Black Bean Burgers</t>
   </si>
   <si>
-    <t xml:space="preserve">coconut oil</t>
+    <t xml:space="preserve">oil coconut</t>
   </si>
   <si>
     <t xml:space="preserve">onion chopped</t>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">onion purple</t>
   </si>
   <si>
-    <t xml:space="preserve">red peper</t>
+    <t xml:space="preserve">red pepper</t>
   </si>
   <si>
     <t xml:space="preserve">2 tsp</t>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">3 cups </t>
   </si>
   <si>
-    <t xml:space="preserve">Tempeh Ratatoullie</t>
+    <t xml:space="preserve">Tempeh Ratatouille</t>
   </si>
   <si>
     <t xml:space="preserve">3 tsbp</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">onion yellow</t>
   </si>
   <si>
-    <t xml:space="preserve">zuchinni</t>
+    <t xml:space="preserve">zucchini</t>
   </si>
   <si>
     <t xml:space="preserve">eggplant</t>
@@ -370,7 +370,7 @@
     <t xml:space="preserve">0.5 qty</t>
   </si>
   <si>
-    <t xml:space="preserve">Chicken Cannellini Soup</t>
+    <t xml:space="preserve">Chicken Cannelloni Soup</t>
   </si>
   <si>
     <t xml:space="preserve">carrots</t>
@@ -433,18 +433,12 @@
     <t xml:space="preserve">spinach</t>
   </si>
   <si>
-    <t xml:space="preserve">parsley</t>
-  </si>
-  <si>
     <t xml:space="preserve">lemon juice</t>
   </si>
   <si>
     <t xml:space="preserve">Chicken Noodle Soup</t>
   </si>
   <si>
-    <t xml:space="preserve">chicken broth</t>
-  </si>
-  <si>
     <t xml:space="preserve">64 oz</t>
   </si>
   <si>
@@ -508,7 +502,7 @@
     <t xml:space="preserve">cardamom</t>
   </si>
   <si>
-    <t xml:space="preserve">thai basil</t>
+    <t xml:space="preserve">basil thai</t>
   </si>
   <si>
     <t xml:space="preserve">bean sprouts</t>
@@ -674,9 +668,9 @@
   <dimension ref="A1:BJ142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A142" activeCellId="0" sqref="A142"/>
+      <selection pane="bottomLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -789,7 +783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -855,7 +849,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
@@ -932,7 +926,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -998,7 +992,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>34</v>
       </c>
@@ -1130,7 +1124,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>51</v>
       </c>
@@ -1949,7 +1943,7 @@
         <v>125</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>136</v>
+        <v>9</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>23</v>
@@ -1960,29 +1954,29 @@
         <v>125</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C112" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>23</v>
@@ -1990,7 +1984,7 @@
     </row>
     <row r="114" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B114" s="4" t="s">
         <v>133</v>
@@ -2001,29 +1995,29 @@
     </row>
     <row r="115" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B115" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>127</v>
@@ -2034,65 +2028,65 @@
     </row>
     <row r="118" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>5</v>
@@ -2100,7 +2094,7 @@
     </row>
     <row r="124" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B124" s="4" t="s">
         <v>131</v>
@@ -2111,7 +2105,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>77</v>
@@ -2122,32 +2116,32 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>55</v>
@@ -2155,10 +2149,10 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>23</v>
@@ -2166,10 +2160,10 @@
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>19</v>
@@ -2177,10 +2171,10 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>29</v>
@@ -2188,10 +2182,10 @@
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B132" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>29</v>
@@ -2199,10 +2193,10 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>24</v>
@@ -2210,10 +2204,10 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>23</v>
@@ -2221,10 +2215,10 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>19</v>
@@ -2232,40 +2226,40 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>59</v>
@@ -2276,10 +2270,10 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>108</v>
@@ -2287,24 +2281,24 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>